<commit_message>
changed revision created plot type
</commit_message>
<xml_diff>
--- a/csv/revision_created_dates.xlsx
+++ b/csv/revision_created_dates.xlsx
@@ -1036,8 +1036,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:areaChart>
-        <c:grouping val="stacked"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1064,6 +1065,7 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>revision_created_dates!$D$2:$D$70</c:f>
@@ -1505,11 +1507,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1526785888"/>
-        <c:axId val="-1526784256"/>
-      </c:areaChart>
+        <c:gapWidth val="30"/>
+        <c:axId val="-665841824"/>
+        <c:axId val="-665852704"/>
+      </c:barChart>
       <c:dateAx>
-        <c:axId val="-1526785888"/>
+        <c:axId val="-665841824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1552,14 +1555,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1526784256"/>
+        <c:crossAx val="-665852704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1526784256"/>
+        <c:axId val="-665852704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,9 +1613,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1526785888"/>
+        <c:crossAx val="-665841824"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2507,8 +2510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="L61" sqref="L61"/>
+    <sheetView tabSelected="1" topLeftCell="G14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>